<commit_message>
Allow ignoring backround colors that won't help
</commit_message>
<xml_diff>
--- a/Benchmark/Compare.xlsx
+++ b/Benchmark/Compare.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boxofyellow/Projects/Ascii3dEngine/Benchmark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B526B96D-7430-3E4C-83CE-829E7794C2D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E52032-3BDB-E342-B2AD-E9542B18C417}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4800" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{DB605785-6E2F-D842-AA87-F2BDEE7FB0D4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Benchmark-Fix Compare" sheetId="4" r:id="rId1"/>
-    <sheet name="Benchmark-1" sheetId="3" r:id="rId2"/>
-    <sheet name="Benchmark-0" sheetId="2" r:id="rId3"/>
-    <sheet name="Org - stop watch" sheetId="1" r:id="rId4"/>
+    <sheet name="Benchmark-IgnoreBackground" sheetId="5" r:id="rId1"/>
+    <sheet name="Benchmark-Fix Compare" sheetId="4" r:id="rId2"/>
+    <sheet name="Benchmark-1" sheetId="3" r:id="rId3"/>
+    <sheet name="Benchmark-0" sheetId="2" r:id="rId4"/>
+    <sheet name="Org - stop watch" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="16">
   <si>
     <t>max Children</t>
   </si>
@@ -148,7 +149,17 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -307,7 +318,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Benchmark-Fix Compare'!$E$2</c:f>
+              <c:f>'Benchmark-IgnoreBackground'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -342,7 +353,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Benchmark-Fix Compare'!$A$3:$A$18</c:f>
+              <c:f>'Benchmark-IgnoreBackground'!$A$3:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -399,7 +410,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Benchmark-Fix Compare'!$E$3:$E$18</c:f>
+              <c:f>'Benchmark-IgnoreBackground'!$E$3:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -407,49 +418,49 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6420580934266096</c:v>
+                  <c:v>1.9010930418555054</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0205680389438732</c:v>
+                  <c:v>1.0918421754198882</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57264902156742636</c:v>
+                  <c:v>0.59554118901626241</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.32580031593539444</c:v>
+                  <c:v>0.33717675286590248</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.20319803991102228</c:v>
+                  <c:v>0.21837509997334045</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.14955349946806795</c:v>
+                  <c:v>0.1563249800053319</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.13108095038524775</c:v>
+                  <c:v>0.13599706744868037</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.12640639607982204</c:v>
+                  <c:v>0.12999866702212742</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.14200973596827751</c:v>
+                  <c:v>0.14666089042921887</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.18656307424481769</c:v>
+                  <c:v>0.19348173820314585</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.22766691382700927</c:v>
+                  <c:v>0.23810317248733673</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.84283826042103227</c:v>
+                  <c:v>0.88892961876832854</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.0198265579161159</c:v>
+                  <c:v>1.0965075979738739</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.0163448209162127</c:v>
+                  <c:v>1.0890429218874969</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.3870530964892485</c:v>
+                  <c:v>8.0780791788856323</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -457,7 +468,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2227-2D47-82A7-D18DD015FC1D}"/>
+              <c16:uniqueId val="{00000000-0279-4742-B2B7-DEBAB787DE3C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -480,7 +491,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Benchmark-Fix Compare'!$G$2</c:f>
+              <c:f>'Benchmark-IgnoreBackground'!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -515,7 +526,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Benchmark-Fix Compare'!$A$3:$A$18</c:f>
+              <c:f>'Benchmark-IgnoreBackground'!$A$3:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -572,7 +583,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Benchmark-Fix Compare'!$G$3:$G$18</c:f>
+              <c:f>'Benchmark-IgnoreBackground'!$G$3:$G$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -580,46 +591,46 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55.71913075421476</c:v>
+                  <c:v>75.130377145242406</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55.716286695852901</c:v>
+                  <c:v>75.12798530346781</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>55.711188010860909</c:v>
+                  <c:v>75.120529440332277</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55.612390656014746</c:v>
+                  <c:v>74.946596950479957</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>55.394170828306606</c:v>
+                  <c:v>74.659514274832489</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>55.008148494607319</c:v>
+                  <c:v>74.361122028143001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>53.870118934010868</c:v>
+                  <c:v>72.800230865205037</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>52.406175880511945</c:v>
+                  <c:v>70.743013765614279</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50.256856579395418</c:v>
+                  <c:v>68.016750853814955</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>46.471562538433759</c:v>
+                  <c:v>62.47875510616015</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44.774903095738722</c:v>
+                  <c:v>60.272480055923516</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.5190536736438887</c:v>
+                  <c:v>11.175554652510222</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.3922938619277323</c:v>
+                  <c:v>9.6411995187386239</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.3922938619277323</c:v>
+                  <c:v>9.6411995187386239</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -630,7 +641,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2227-2D47-82A7-D18DD015FC1D}"/>
+              <c16:uniqueId val="{00000001-0279-4742-B2B7-DEBAB787DE3C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1005,7 +1016,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Benchmark-0'!$E$2</c:f>
+              <c:f>'Benchmark-Fix Compare'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1040,7 +1051,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Benchmark-0'!$A$3:$A$18</c:f>
+              <c:f>'Benchmark-Fix Compare'!$A$3:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1097,7 +1108,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Benchmark-0'!$E$3:$E$18</c:f>
+              <c:f>'Benchmark-Fix Compare'!$E$3:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1105,49 +1116,49 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6949940439873326</c:v>
+                  <c:v>1.6420580934266096</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0358522908858478</c:v>
+                  <c:v>1.0205680389438732</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.51390220517737295</c:v>
+                  <c:v>0.57264902156742636</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.27682384729364595</c:v>
+                  <c:v>0.32580031593539444</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.18321276039396844</c:v>
+                  <c:v>0.20319803991102228</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.14907463900752493</c:v>
+                  <c:v>0.14955349946806795</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.14773816787239608</c:v>
+                  <c:v>0.13108095038524775</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.17754728492983526</c:v>
+                  <c:v>0.12640639607982204</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.23205206426682939</c:v>
+                  <c:v>0.14200973596827751</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.35006827624277287</c:v>
+                  <c:v>0.18656307424481769</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.3986170429123449</c:v>
+                  <c:v>0.22766691382700927</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.85603881577035934</c:v>
+                  <c:v>0.84283826042103227</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.1698480490426799</c:v>
+                  <c:v>1.0198265579161159</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.0309131584299369</c:v>
+                  <c:v>1.0163448209162127</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8.755977802957668</c:v>
+                  <c:v>7.3870530964892485</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1155,7 +1166,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2803-F747-B975-326804F98C39}"/>
+              <c16:uniqueId val="{00000000-2227-2D47-82A7-D18DD015FC1D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1178,7 +1189,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Benchmark-0'!$G$2</c:f>
+              <c:f>'Benchmark-Fix Compare'!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1213,7 +1224,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Benchmark-0'!$A$3:$A$18</c:f>
+              <c:f>'Benchmark-Fix Compare'!$A$3:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1270,7 +1281,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Benchmark-0'!$G$3:$G$18</c:f>
+              <c:f>'Benchmark-Fix Compare'!$G$3:$G$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1278,46 +1289,46 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>98.404034733567556</c:v>
+                  <c:v>55.71913075421476</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>98.235459109266131</c:v>
+                  <c:v>55.716286695852901</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98.233997674220674</c:v>
+                  <c:v>55.711188010860909</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>97.013468877933761</c:v>
+                  <c:v>55.612390656014746</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>91.288483051946173</c:v>
+                  <c:v>55.394170828306606</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>90.271434597823557</c:v>
+                  <c:v>55.008148494607319</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>88.928756251136306</c:v>
+                  <c:v>53.870118934010868</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>81.024710093666101</c:v>
+                  <c:v>52.406175880511945</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>63.115721335025931</c:v>
+                  <c:v>50.256856579395418</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42.70115925125949</c:v>
+                  <c:v>46.471562538433759</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34.059361638859471</c:v>
+                  <c:v>44.774903095738722</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.4701384253723315</c:v>
+                  <c:v>8.5190536736438887</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.7941348025446291</c:v>
+                  <c:v>7.3922938619277323</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.7941348025446291</c:v>
+                  <c:v>7.3922938619277323</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -1328,7 +1339,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2803-F747-B975-326804F98C39}"/>
+              <c16:uniqueId val="{00000001-2227-2D47-82A7-D18DD015FC1D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1653,6 +1664,704 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>C Search &amp;</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> C Avg vs Max Children</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark-0'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C Search</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Benchmark-0'!$A$3:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16384</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Benchmark-0'!$E$3:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6949940439873326</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0358522908858478</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.51390220517737295</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.27682384729364595</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.18321276039396844</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.14907463900752493</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.14773816787239608</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.17754728492983526</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.23205206426682939</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.35006827624277287</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.3986170429123449</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.85603881577035934</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1698480490426799</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0309131584299369</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.755977802957668</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2803-F747-B975-326804F98C39}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="200140560"/>
+        <c:axId val="1829147359"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark-0'!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C Avg Dif</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Benchmark-0'!$A$3:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16384</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Benchmark-0'!$G$3:$G$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>98.404034733567556</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>98.235459109266131</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98.233997674220674</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97.013468877933761</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>91.288483051946173</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90.271434597823557</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>88.928756251136306</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>81.024710093666101</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>63.115721335025931</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42.70115925125949</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>34.059361638859471</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.4701384253723315</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.7941348025446291</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.7941348025446291</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2803-F747-B975-326804F98C39}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1830783935"/>
+        <c:axId val="199545920"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="200140560"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="10000"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1829147359"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1829147359"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="200140560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="199545920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1830783935"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1830783935"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="199545920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>Time</a:t>
             </a:r>
             <a:r>
@@ -2304,7 +3013,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2905,7 +3614,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3589,7 +4298,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4431,6 +5140,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -7527,7 +8276,566 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{310D69AC-5546-E54B-8C12-154841A04AC6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7570,7 +8878,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7611,7 +8919,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8056,10 +9364,467 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCEB006D-EF5F-2D4D-86DC-4D6E506A45E0}">
+  <dimension ref="A2:L18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0.5</v>
+      </c>
+      <c r="B3">
+        <v>300.08</v>
+      </c>
+      <c r="C3">
+        <v>1.26138969316015</v>
+      </c>
+      <c r="D3">
+        <v>6.3556460153053093E-2</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:G18" si="0">B3/B$3</f>
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>570.48</v>
+      </c>
+      <c r="C4">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D4">
+        <v>4.7750208213154499</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>1.9010930418555054</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>75.130377145242406</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>327.64</v>
+      </c>
+      <c r="C5">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D5">
+        <v>4.7748688043190102</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>1.0918421754198882</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>75.12798530346781</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>178.71</v>
+      </c>
+      <c r="C6">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D6">
+        <v>4.7743949360507303</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.59554118901626241</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>75.120529440332277</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>101.18</v>
+      </c>
+      <c r="C7">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D7">
+        <v>4.7633404026901101</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.33717675286590248</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>74.946596950479957</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>65.53</v>
+      </c>
+      <c r="C8">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D8">
+        <v>4.7450944440546898</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.21837509997334045</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>74.659514274832489</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>32</v>
+      </c>
+      <c r="B9">
+        <v>46.91</v>
+      </c>
+      <c r="C9">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D9">
+        <v>4.7261296891179896</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.1563249800053319</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>74.361122028143001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>64</v>
+      </c>
+      <c r="B10">
+        <v>40.81</v>
+      </c>
+      <c r="C10">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D10">
+        <v>4.6269249721174699</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.13599706744868037</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>72.800230865205037</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>128</v>
+      </c>
+      <c r="B11">
+        <v>39.01</v>
+      </c>
+      <c r="C11">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D11">
+        <v>4.4961755355011501</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0.12999866702212742</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>70.743013765614279</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>256</v>
+      </c>
+      <c r="B12">
+        <v>44.01</v>
+      </c>
+      <c r="C12">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D12">
+        <v>4.3229039153806301</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0.14666089042921887</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>68.016750853814955</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>512</v>
+      </c>
+      <c r="B13">
+        <v>58.06</v>
+      </c>
+      <c r="C13">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D13">
+        <v>3.9709285093170301</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0.19348173820314585</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>62.47875510616015</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1024</v>
+      </c>
+      <c r="B14">
+        <v>71.45</v>
+      </c>
+      <c r="C14">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D14">
+        <v>3.8307054769999902</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0.23810317248733673</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>60.272480055923516</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2048</v>
+      </c>
+      <c r="B15">
+        <v>266.75</v>
+      </c>
+      <c r="C15">
+        <v>55.8877226475811</v>
+      </c>
+      <c r="D15">
+        <v>0.710278693960533</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0.88892961876832854</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>44.306468453508614</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>11.175554652510222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>4096</v>
+      </c>
+      <c r="B16">
+        <v>329.04</v>
+      </c>
+      <c r="C16">
+        <v>55.8877226475811</v>
+      </c>
+      <c r="D16">
+        <v>0.61276051304034596</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>1.0965075979738739</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>44.306468453508614</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>9.6411995187386239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>8192</v>
+      </c>
+      <c r="B17">
+        <v>326.8</v>
+      </c>
+      <c r="C17">
+        <v>55.8877226475811</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0.61276051304034596</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>1.0890429218874969</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>44.306468453508614</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>9.6411995187386239</v>
+      </c>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>16384</v>
+      </c>
+      <c r="B18" s="5">
+        <v>2424.0700000000002</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>8.0780791788856323</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B4:B18">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>$B$3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B42892-40D1-4548-A56D-9001ACB7B0BC}">
   <dimension ref="A2:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -8519,7 +10284,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B4:B18">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
       <formula>$B$3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8528,7 +10293,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC69C5D9-B88F-FF4D-BBBE-0229262C4A41}">
   <dimension ref="A1:L18"/>
   <sheetViews>
@@ -8997,7 +10762,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B4:B18">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>$B$3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9005,7 +10770,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393E3666-8983-354A-B652-1578FACF0E70}">
   <dimension ref="A1:G18"/>
   <sheetViews>
@@ -9457,7 +11222,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B4:B18">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
       <formula>$B$3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9466,7 +11231,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310253C2-5867-A04F-B696-06BC56F172E8}">
   <dimension ref="A1:U17"/>
   <sheetViews>
@@ -10633,17 +12398,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J2:J16">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>$C$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K16">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M16">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Use a 4-way split. Zoom zoom
</commit_message>
<xml_diff>
--- a/Benchmark/Compare.xlsx
+++ b/Benchmark/Compare.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boxofyellow/Projects/Ascii3dEngine/Benchmark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E52032-3BDB-E342-B2AD-E9542B18C417}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173693A0-7737-714F-8B09-B8A4FC32072B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4800" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{DB605785-6E2F-D842-AA87-F2BDEE7FB0D4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Benchmark-IgnoreBackground" sheetId="5" r:id="rId1"/>
-    <sheet name="Benchmark-Fix Compare" sheetId="4" r:id="rId2"/>
-    <sheet name="Benchmark-1" sheetId="3" r:id="rId3"/>
-    <sheet name="Benchmark-0" sheetId="2" r:id="rId4"/>
-    <sheet name="Org - stop watch" sheetId="1" r:id="rId5"/>
+    <sheet name="Benchmark-SplitBy4" sheetId="6" r:id="rId1"/>
+    <sheet name="Benchmark-IgnoreBackground" sheetId="5" r:id="rId2"/>
+    <sheet name="Benchmark-Fix Compare" sheetId="4" r:id="rId3"/>
+    <sheet name="Benchmark-1" sheetId="3" r:id="rId4"/>
+    <sheet name="Benchmark-0" sheetId="2" r:id="rId5"/>
+    <sheet name="Org - stop watch" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="16">
   <si>
     <t>max Children</t>
   </si>
@@ -149,7 +150,17 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -318,7 +329,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Benchmark-IgnoreBackground'!$E$2</c:f>
+              <c:f>'Benchmark-SplitBy4'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -353,7 +364,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Benchmark-IgnoreBackground'!$A$3:$A$18</c:f>
+              <c:f>'Benchmark-SplitBy4'!$A$3:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -410,7 +421,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Benchmark-IgnoreBackground'!$E$3:$E$18</c:f>
+              <c:f>'Benchmark-SplitBy4'!$E$3:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -418,49 +429,49 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9010930418555054</c:v>
+                  <c:v>2.691465877600864</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0918421754198882</c:v>
+                  <c:v>1.5482598280963786</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.59554118901626241</c:v>
+                  <c:v>0.84040204781363026</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.33717675286590248</c:v>
+                  <c:v>0.47217134000281813</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.21837509997334045</c:v>
+                  <c:v>0.30576299845004928</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.1563249800053319</c:v>
+                  <c:v>0.22131417030670236</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.13599706744868037</c:v>
+                  <c:v>0.19383777182847214</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.12999866702212742</c:v>
+                  <c:v>0.18129726175379268</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.14666089042921887</c:v>
+                  <c:v>0.20590859987788268</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.19348173820314585</c:v>
+                  <c:v>0.27467004837724857</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.23810317248733673</c:v>
+                  <c:v>0.33535296604198961</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.88892961876832854</c:v>
+                  <c:v>1.2496359964304167</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.0965075979738739</c:v>
+                  <c:v>1.5384434737682591</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.0890429218874969</c:v>
+                  <c:v>1.5351087313888496</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8.0780791788856323</c:v>
+                  <c:v>11.377812221126296</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -468,7 +479,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0279-4742-B2B7-DEBAB787DE3C}"/>
+              <c16:uniqueId val="{00000000-FB93-F54A-AE72-567299124932}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -491,7 +502,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Benchmark-IgnoreBackground'!$G$2</c:f>
+              <c:f>'Benchmark-SplitBy4'!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -526,7 +537,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Benchmark-IgnoreBackground'!$A$3:$A$18</c:f>
+              <c:f>'Benchmark-SplitBy4'!$A$3:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -583,7 +594,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Benchmark-IgnoreBackground'!$G$3:$G$18</c:f>
+              <c:f>'Benchmark-SplitBy4'!$G$3:$G$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -641,7 +652,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0279-4742-B2B7-DEBAB787DE3C}"/>
+              <c16:uniqueId val="{00000001-FB93-F54A-AE72-567299124932}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1016,7 +1027,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Benchmark-Fix Compare'!$E$2</c:f>
+              <c:f>'Benchmark-IgnoreBackground'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1051,7 +1062,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Benchmark-Fix Compare'!$A$3:$A$18</c:f>
+              <c:f>'Benchmark-IgnoreBackground'!$A$3:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1108,7 +1119,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Benchmark-Fix Compare'!$E$3:$E$18</c:f>
+              <c:f>'Benchmark-IgnoreBackground'!$E$3:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1116,49 +1127,49 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6420580934266096</c:v>
+                  <c:v>1.9010930418555054</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0205680389438732</c:v>
+                  <c:v>1.0918421754198882</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57264902156742636</c:v>
+                  <c:v>0.59554118901626241</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.32580031593539444</c:v>
+                  <c:v>0.33717675286590248</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.20319803991102228</c:v>
+                  <c:v>0.21837509997334045</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.14955349946806795</c:v>
+                  <c:v>0.1563249800053319</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.13108095038524775</c:v>
+                  <c:v>0.13599706744868037</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.12640639607982204</c:v>
+                  <c:v>0.12999866702212742</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.14200973596827751</c:v>
+                  <c:v>0.14666089042921887</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.18656307424481769</c:v>
+                  <c:v>0.19348173820314585</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.22766691382700927</c:v>
+                  <c:v>0.23810317248733673</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.84283826042103227</c:v>
+                  <c:v>0.88892961876832854</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.0198265579161159</c:v>
+                  <c:v>1.0965075979738739</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.0163448209162127</c:v>
+                  <c:v>1.0890429218874969</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.3870530964892485</c:v>
+                  <c:v>8.0780791788856323</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1166,7 +1177,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2227-2D47-82A7-D18DD015FC1D}"/>
+              <c16:uniqueId val="{00000000-0279-4742-B2B7-DEBAB787DE3C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1189,7 +1200,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Benchmark-Fix Compare'!$G$2</c:f>
+              <c:f>'Benchmark-IgnoreBackground'!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1224,7 +1235,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Benchmark-Fix Compare'!$A$3:$A$18</c:f>
+              <c:f>'Benchmark-IgnoreBackground'!$A$3:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1281,7 +1292,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Benchmark-Fix Compare'!$G$3:$G$18</c:f>
+              <c:f>'Benchmark-IgnoreBackground'!$G$3:$G$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1289,46 +1300,46 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55.71913075421476</c:v>
+                  <c:v>75.130377145242406</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55.716286695852901</c:v>
+                  <c:v>75.12798530346781</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>55.711188010860909</c:v>
+                  <c:v>75.120529440332277</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55.612390656014746</c:v>
+                  <c:v>74.946596950479957</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>55.394170828306606</c:v>
+                  <c:v>74.659514274832489</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>55.008148494607319</c:v>
+                  <c:v>74.361122028143001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>53.870118934010868</c:v>
+                  <c:v>72.800230865205037</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>52.406175880511945</c:v>
+                  <c:v>70.743013765614279</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50.256856579395418</c:v>
+                  <c:v>68.016750853814955</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>46.471562538433759</c:v>
+                  <c:v>62.47875510616015</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44.774903095738722</c:v>
+                  <c:v>60.272480055923516</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.5190536736438887</c:v>
+                  <c:v>11.175554652510222</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.3922938619277323</c:v>
+                  <c:v>9.6411995187386239</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.3922938619277323</c:v>
+                  <c:v>9.6411995187386239</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -1339,7 +1350,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2227-2D47-82A7-D18DD015FC1D}"/>
+              <c16:uniqueId val="{00000001-0279-4742-B2B7-DEBAB787DE3C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1714,7 +1725,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Benchmark-0'!$E$2</c:f>
+              <c:f>'Benchmark-Fix Compare'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1749,7 +1760,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Benchmark-0'!$A$3:$A$18</c:f>
+              <c:f>'Benchmark-Fix Compare'!$A$3:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1806,7 +1817,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Benchmark-0'!$E$3:$E$18</c:f>
+              <c:f>'Benchmark-Fix Compare'!$E$3:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1814,49 +1825,49 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6949940439873326</c:v>
+                  <c:v>1.6420580934266096</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0358522908858478</c:v>
+                  <c:v>1.0205680389438732</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.51390220517737295</c:v>
+                  <c:v>0.57264902156742636</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.27682384729364595</c:v>
+                  <c:v>0.32580031593539444</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.18321276039396844</c:v>
+                  <c:v>0.20319803991102228</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.14907463900752493</c:v>
+                  <c:v>0.14955349946806795</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.14773816787239608</c:v>
+                  <c:v>0.13108095038524775</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.17754728492983526</c:v>
+                  <c:v>0.12640639607982204</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.23205206426682939</c:v>
+                  <c:v>0.14200973596827751</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.35006827624277287</c:v>
+                  <c:v>0.18656307424481769</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.3986170429123449</c:v>
+                  <c:v>0.22766691382700927</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.85603881577035934</c:v>
+                  <c:v>0.84283826042103227</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.1698480490426799</c:v>
+                  <c:v>1.0198265579161159</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.0309131584299369</c:v>
+                  <c:v>1.0163448209162127</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8.755977802957668</c:v>
+                  <c:v>7.3870530964892485</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1864,7 +1875,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2803-F747-B975-326804F98C39}"/>
+              <c16:uniqueId val="{00000000-2227-2D47-82A7-D18DD015FC1D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1887,7 +1898,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Benchmark-0'!$G$2</c:f>
+              <c:f>'Benchmark-Fix Compare'!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1922,7 +1933,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Benchmark-0'!$A$3:$A$18</c:f>
+              <c:f>'Benchmark-Fix Compare'!$A$3:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1979,7 +1990,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Benchmark-0'!$G$3:$G$18</c:f>
+              <c:f>'Benchmark-Fix Compare'!$G$3:$G$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1987,46 +1998,46 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>98.404034733567556</c:v>
+                  <c:v>55.71913075421476</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>98.235459109266131</c:v>
+                  <c:v>55.716286695852901</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98.233997674220674</c:v>
+                  <c:v>55.711188010860909</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>97.013468877933761</c:v>
+                  <c:v>55.612390656014746</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>91.288483051946173</c:v>
+                  <c:v>55.394170828306606</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>90.271434597823557</c:v>
+                  <c:v>55.008148494607319</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>88.928756251136306</c:v>
+                  <c:v>53.870118934010868</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>81.024710093666101</c:v>
+                  <c:v>52.406175880511945</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>63.115721335025931</c:v>
+                  <c:v>50.256856579395418</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42.70115925125949</c:v>
+                  <c:v>46.471562538433759</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34.059361638859471</c:v>
+                  <c:v>44.774903095738722</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.4701384253723315</c:v>
+                  <c:v>8.5190536736438887</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.7941348025446291</c:v>
+                  <c:v>7.3922938619277323</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.7941348025446291</c:v>
+                  <c:v>7.3922938619277323</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -2037,7 +2048,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2803-F747-B975-326804F98C39}"/>
+              <c16:uniqueId val="{00000001-2227-2D47-82A7-D18DD015FC1D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2362,6 +2373,704 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>C Search &amp;</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> C Avg vs Max Children</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark-0'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C Search</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Benchmark-0'!$A$3:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16384</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Benchmark-0'!$E$3:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6949940439873326</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0358522908858478</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.51390220517737295</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.27682384729364595</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.18321276039396844</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.14907463900752493</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.14773816787239608</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.17754728492983526</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.23205206426682939</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.35006827624277287</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.3986170429123449</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.85603881577035934</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1698480490426799</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0309131584299369</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.755977802957668</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2803-F747-B975-326804F98C39}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="200140560"/>
+        <c:axId val="1829147359"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark-0'!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C Avg Dif</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Benchmark-0'!$A$3:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16384</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Benchmark-0'!$G$3:$G$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>98.404034733567556</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>98.235459109266131</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98.233997674220674</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97.013468877933761</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>91.288483051946173</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90.271434597823557</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>88.928756251136306</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>81.024710093666101</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>63.115721335025931</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42.70115925125949</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>34.059361638859471</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.4701384253723315</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.7941348025446291</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.7941348025446291</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2803-F747-B975-326804F98C39}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1830783935"/>
+        <c:axId val="199545920"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="200140560"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="10000"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1829147359"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1829147359"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="200140560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="199545920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1830783935"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1830783935"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="199545920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>Time</a:t>
             </a:r>
             <a:r>
@@ -3013,7 +3722,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3614,7 +4323,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4298,7 +5007,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5180,6 +5889,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -8792,7 +9541,566 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7760DA6D-D0CE-054A-9373-C6DA3B7EEEEF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8835,7 +10143,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8878,7 +10186,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8919,7 +10227,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -9364,7 +10672,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCEB006D-EF5F-2D4D-86DC-4D6E506A45E0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7AEF0CA-7BED-8C47-B9D6-5A56E6D2CDD3}">
   <dimension ref="A2:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -9397,7 +10705,7 @@
         <v>0.5</v>
       </c>
       <c r="B3">
-        <v>300.08</v>
+        <v>212.91</v>
       </c>
       <c r="C3">
         <v>1.26138969316015</v>
@@ -9423,7 +10731,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>570.48</v>
+        <v>573.04</v>
       </c>
       <c r="C4">
         <v>82.538015905202897</v>
@@ -9433,7 +10741,7 @@
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>1.9010930418555054</v>
+        <v>2.691465877600864</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
@@ -9449,7 +10757,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>327.64</v>
+        <v>329.64</v>
       </c>
       <c r="C5">
         <v>82.538015905202897</v>
@@ -9459,7 +10767,7 @@
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>1.0918421754198882</v>
+        <v>1.5482598280963786</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
@@ -9475,7 +10783,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>178.71</v>
+        <v>178.93</v>
       </c>
       <c r="C6">
         <v>82.538015905202897</v>
@@ -9485,7 +10793,7 @@
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>0.59554118901626241</v>
+        <v>0.84040204781363026</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
@@ -9501,7 +10809,7 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>101.18</v>
+        <v>100.53</v>
       </c>
       <c r="C7">
         <v>82.538015905202897</v>
@@ -9511,7 +10819,7 @@
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>0.33717675286590248</v>
+        <v>0.47217134000281813</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
@@ -9527,7 +10835,7 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>65.53</v>
+        <v>65.099999999999994</v>
       </c>
       <c r="C8">
         <v>82.538015905202897</v>
@@ -9537,7 +10845,7 @@
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>0.21837509997334045</v>
+        <v>0.30576299845004928</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
@@ -9553,7 +10861,7 @@
         <v>32</v>
       </c>
       <c r="B9">
-        <v>46.91</v>
+        <v>47.12</v>
       </c>
       <c r="C9">
         <v>82.538015905202897</v>
@@ -9563,7 +10871,7 @@
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0.1563249800053319</v>
+        <v>0.22131417030670236</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
@@ -9579,7 +10887,7 @@
         <v>64</v>
       </c>
       <c r="B10">
-        <v>40.81</v>
+        <v>41.27</v>
       </c>
       <c r="C10">
         <v>82.538015905202897</v>
@@ -9589,7 +10897,7 @@
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>0.13599706744868037</v>
+        <v>0.19383777182847214</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
@@ -9605,7 +10913,7 @@
         <v>128</v>
       </c>
       <c r="B11">
-        <v>39.01</v>
+        <v>38.6</v>
       </c>
       <c r="C11">
         <v>82.538015905202897</v>
@@ -9615,7 +10923,7 @@
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>0.12999866702212742</v>
+        <v>0.18129726175379268</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
@@ -9631,7 +10939,7 @@
         <v>256</v>
       </c>
       <c r="B12">
-        <v>44.01</v>
+        <v>43.84</v>
       </c>
       <c r="C12">
         <v>82.538015905202897</v>
@@ -9641,7 +10949,7 @@
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>0.14666089042921887</v>
+        <v>0.20590859987788268</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
@@ -9657,7 +10965,7 @@
         <v>512</v>
       </c>
       <c r="B13">
-        <v>58.06</v>
+        <v>58.48</v>
       </c>
       <c r="C13">
         <v>82.538015905202897</v>
@@ -9667,7 +10975,7 @@
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>0.19348173820314585</v>
+        <v>0.27467004837724857</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
@@ -9683,7 +10991,7 @@
         <v>1024</v>
       </c>
       <c r="B14">
-        <v>71.45</v>
+        <v>71.400000000000006</v>
       </c>
       <c r="C14">
         <v>82.538015905202897</v>
@@ -9693,7 +11001,7 @@
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>0.23810317248733673</v>
+        <v>0.33535296604198961</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
@@ -9709,7 +11017,7 @@
         <v>2048</v>
       </c>
       <c r="B15">
-        <v>266.75</v>
+        <v>266.06</v>
       </c>
       <c r="C15">
         <v>55.8877226475811</v>
@@ -9719,7 +11027,7 @@
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>0.88892961876832854</v>
+        <v>1.2496359964304167</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
@@ -9735,7 +11043,7 @@
         <v>4096</v>
       </c>
       <c r="B16">
-        <v>329.04</v>
+        <v>327.55</v>
       </c>
       <c r="C16">
         <v>55.8877226475811</v>
@@ -9745,7 +11053,7 @@
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>1.0965075979738739</v>
+        <v>1.5384434737682591</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
@@ -9761,7 +11069,7 @@
         <v>8192</v>
       </c>
       <c r="B17">
-        <v>326.8</v>
+        <v>326.83999999999997</v>
       </c>
       <c r="C17">
         <v>55.8877226475811</v>
@@ -9771,7 +11079,7 @@
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>1.0890429218874969</v>
+        <v>1.5351087313888496</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
@@ -9788,7 +11096,7 @@
         <v>16384</v>
       </c>
       <c r="B18" s="5">
-        <v>2424.0700000000002</v>
+        <v>2422.4499999999998</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -9798,7 +11106,7 @@
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>8.0780791788856323</v>
+        <v>11.377812221126296</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
@@ -9808,6 +11116,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="L18" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B4:B18">
@@ -9821,6 +11130,463 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCEB006D-EF5F-2D4D-86DC-4D6E506A45E0}">
+  <dimension ref="A2:L18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0.5</v>
+      </c>
+      <c r="B3">
+        <v>300.08</v>
+      </c>
+      <c r="C3">
+        <v>1.26138969316015</v>
+      </c>
+      <c r="D3">
+        <v>6.3556460153053093E-2</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:G18" si="0">B3/B$3</f>
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>570.48</v>
+      </c>
+      <c r="C4">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D4">
+        <v>4.7750208213154499</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>1.9010930418555054</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>75.130377145242406</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>327.64</v>
+      </c>
+      <c r="C5">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D5">
+        <v>4.7748688043190102</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>1.0918421754198882</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>75.12798530346781</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>178.71</v>
+      </c>
+      <c r="C6">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D6">
+        <v>4.7743949360507303</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.59554118901626241</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>75.120529440332277</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>101.18</v>
+      </c>
+      <c r="C7">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D7">
+        <v>4.7633404026901101</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.33717675286590248</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>74.946596950479957</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>65.53</v>
+      </c>
+      <c r="C8">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D8">
+        <v>4.7450944440546898</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.21837509997334045</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>74.659514274832489</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>32</v>
+      </c>
+      <c r="B9">
+        <v>46.91</v>
+      </c>
+      <c r="C9">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D9">
+        <v>4.7261296891179896</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.1563249800053319</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>74.361122028143001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>64</v>
+      </c>
+      <c r="B10">
+        <v>40.81</v>
+      </c>
+      <c r="C10">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D10">
+        <v>4.6269249721174699</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.13599706744868037</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>72.800230865205037</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>128</v>
+      </c>
+      <c r="B11">
+        <v>39.01</v>
+      </c>
+      <c r="C11">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D11">
+        <v>4.4961755355011501</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0.12999866702212742</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>70.743013765614279</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>256</v>
+      </c>
+      <c r="B12">
+        <v>44.01</v>
+      </c>
+      <c r="C12">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D12">
+        <v>4.3229039153806301</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0.14666089042921887</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>68.016750853814955</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>512</v>
+      </c>
+      <c r="B13">
+        <v>58.06</v>
+      </c>
+      <c r="C13">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D13">
+        <v>3.9709285093170301</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0.19348173820314585</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>62.47875510616015</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1024</v>
+      </c>
+      <c r="B14">
+        <v>71.45</v>
+      </c>
+      <c r="C14">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D14">
+        <v>3.8307054769999902</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0.23810317248733673</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>60.272480055923516</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2048</v>
+      </c>
+      <c r="B15">
+        <v>266.75</v>
+      </c>
+      <c r="C15">
+        <v>55.8877226475811</v>
+      </c>
+      <c r="D15">
+        <v>0.710278693960533</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0.88892961876832854</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>44.306468453508614</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>11.175554652510222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>4096</v>
+      </c>
+      <c r="B16">
+        <v>329.04</v>
+      </c>
+      <c r="C16">
+        <v>55.8877226475811</v>
+      </c>
+      <c r="D16">
+        <v>0.61276051304034596</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>1.0965075979738739</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>44.306468453508614</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>9.6411995187386239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>8192</v>
+      </c>
+      <c r="B17">
+        <v>326.8</v>
+      </c>
+      <c r="C17">
+        <v>55.8877226475811</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0.61276051304034596</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>1.0890429218874969</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>44.306468453508614</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>9.6411995187386239</v>
+      </c>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>16384</v>
+      </c>
+      <c r="B18" s="5">
+        <v>2424.0700000000002</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>8.0780791788856323</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B4:B18">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
+      <formula>$B$3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B42892-40D1-4548-A56D-9001ACB7B0BC}">
   <dimension ref="A2:I18"/>
   <sheetViews>
@@ -10293,7 +12059,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC69C5D9-B88F-FF4D-BBBE-0229262C4A41}">
   <dimension ref="A1:L18"/>
   <sheetViews>
@@ -10770,7 +12536,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393E3666-8983-354A-B652-1578FACF0E70}">
   <dimension ref="A1:G18"/>
   <sheetViews>
@@ -11231,7 +12997,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310253C2-5867-A04F-B696-06BC56F172E8}">
   <dimension ref="A1:U17"/>
   <sheetViews>

</xml_diff>

<commit_message>
Allow ignoring foreground colors that won't help
</commit_message>
<xml_diff>
--- a/Benchmark/Compare.xlsx
+++ b/Benchmark/Compare.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boxofyellow/Projects/Ascii3dEngine/Benchmark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173693A0-7737-714F-8B09-B8A4FC32072B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C773226-4A05-6141-9260-6EFE5CB9855C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4800" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{DB605785-6E2F-D842-AA87-F2BDEE7FB0D4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Benchmark-SplitBy4" sheetId="6" r:id="rId1"/>
-    <sheet name="Benchmark-IgnoreBackground" sheetId="5" r:id="rId2"/>
-    <sheet name="Benchmark-Fix Compare" sheetId="4" r:id="rId3"/>
-    <sheet name="Benchmark-1" sheetId="3" r:id="rId4"/>
-    <sheet name="Benchmark-0" sheetId="2" r:id="rId5"/>
-    <sheet name="Org - stop watch" sheetId="1" r:id="rId6"/>
+    <sheet name="Benchmark-IgnoreForeground" sheetId="7" r:id="rId1"/>
+    <sheet name="Benchmark-SplitBy4" sheetId="6" r:id="rId2"/>
+    <sheet name="Benchmark-IgnoreBackground" sheetId="5" r:id="rId3"/>
+    <sheet name="Benchmark-Fix Compare" sheetId="4" r:id="rId4"/>
+    <sheet name="Benchmark-1" sheetId="3" r:id="rId5"/>
+    <sheet name="Benchmark-0" sheetId="2" r:id="rId6"/>
+    <sheet name="Org - stop watch" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="16">
   <si>
     <t>max Children</t>
   </si>
@@ -150,7 +151,17 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -329,7 +340,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Benchmark-SplitBy4'!$E$2</c:f>
+              <c:f>'Benchmark-IgnoreForeground'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -364,7 +375,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Benchmark-SplitBy4'!$A$3:$A$18</c:f>
+              <c:f>'Benchmark-IgnoreForeground'!$A$3:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -421,7 +432,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Benchmark-SplitBy4'!$E$3:$E$18</c:f>
+              <c:f>'Benchmark-IgnoreForeground'!$E$3:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -429,49 +440,49 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.691465877600864</c:v>
+                  <c:v>3.0032623101233558</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5482598280963786</c:v>
+                  <c:v>1.7332042002242836</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.84040204781363026</c:v>
+                  <c:v>0.9395962891222347</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.47217134000281813</c:v>
+                  <c:v>0.54149250688143546</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.30576299845004928</c:v>
+                  <c:v>0.34366398205729431</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.22131417030670236</c:v>
+                  <c:v>0.24701804465286981</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.19383777182847214</c:v>
+                  <c:v>0.21653583443776123</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.18129726175379268</c:v>
+                  <c:v>0.20114180854317462</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.20590859987788268</c:v>
+                  <c:v>0.2340707513508003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.27467004837724857</c:v>
+                  <c:v>0.31420124375573449</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.33535296604198961</c:v>
+                  <c:v>0.374044245081048</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.2496359964304167</c:v>
+                  <c:v>1.396472627179121</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.5384434737682591</c:v>
+                  <c:v>1.7095014782342746</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.5351087313888496</c:v>
+                  <c:v>1.7233662962585379</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11.377812221126296</c:v>
+                  <c:v>12.368997859108982</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -479,7 +490,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FB93-F54A-AE72-567299124932}"/>
+              <c16:uniqueId val="{00000000-E670-C045-87BB-547FEB129655}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -502,7 +513,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Benchmark-SplitBy4'!$G$2</c:f>
+              <c:f>'Benchmark-IgnoreForeground'!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -537,7 +548,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Benchmark-SplitBy4'!$A$3:$A$18</c:f>
+              <c:f>'Benchmark-IgnoreForeground'!$A$3:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -594,7 +605,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Benchmark-SplitBy4'!$G$3:$G$18</c:f>
+              <c:f>'Benchmark-IgnoreForeground'!$G$3:$G$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -652,7 +663,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-FB93-F54A-AE72-567299124932}"/>
+              <c16:uniqueId val="{00000001-E670-C045-87BB-547FEB129655}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1027,7 +1038,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Benchmark-IgnoreBackground'!$E$2</c:f>
+              <c:f>'Benchmark-SplitBy4'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1062,7 +1073,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Benchmark-IgnoreBackground'!$A$3:$A$18</c:f>
+              <c:f>'Benchmark-SplitBy4'!$A$3:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1119,7 +1130,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Benchmark-IgnoreBackground'!$E$3:$E$18</c:f>
+              <c:f>'Benchmark-SplitBy4'!$E$3:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1127,49 +1138,49 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9010930418555054</c:v>
+                  <c:v>2.691465877600864</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0918421754198882</c:v>
+                  <c:v>1.5482598280963786</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.59554118901626241</c:v>
+                  <c:v>0.84040204781363026</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.33717675286590248</c:v>
+                  <c:v>0.47217134000281813</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.21837509997334045</c:v>
+                  <c:v>0.30576299845004928</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.1563249800053319</c:v>
+                  <c:v>0.22131417030670236</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.13599706744868037</c:v>
+                  <c:v>0.19383777182847214</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.12999866702212742</c:v>
+                  <c:v>0.18129726175379268</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.14666089042921887</c:v>
+                  <c:v>0.20590859987788268</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.19348173820314585</c:v>
+                  <c:v>0.27467004837724857</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.23810317248733673</c:v>
+                  <c:v>0.33535296604198961</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.88892961876832854</c:v>
+                  <c:v>1.2496359964304167</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.0965075979738739</c:v>
+                  <c:v>1.5384434737682591</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.0890429218874969</c:v>
+                  <c:v>1.5351087313888496</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8.0780791788856323</c:v>
+                  <c:v>11.377812221126296</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1177,7 +1188,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0279-4742-B2B7-DEBAB787DE3C}"/>
+              <c16:uniqueId val="{00000000-FB93-F54A-AE72-567299124932}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1200,7 +1211,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Benchmark-IgnoreBackground'!$G$2</c:f>
+              <c:f>'Benchmark-SplitBy4'!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1235,7 +1246,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Benchmark-IgnoreBackground'!$A$3:$A$18</c:f>
+              <c:f>'Benchmark-SplitBy4'!$A$3:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1292,7 +1303,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Benchmark-IgnoreBackground'!$G$3:$G$18</c:f>
+              <c:f>'Benchmark-SplitBy4'!$G$3:$G$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1350,7 +1361,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0279-4742-B2B7-DEBAB787DE3C}"/>
+              <c16:uniqueId val="{00000001-FB93-F54A-AE72-567299124932}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1725,7 +1736,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Benchmark-Fix Compare'!$E$2</c:f>
+              <c:f>'Benchmark-IgnoreBackground'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1760,7 +1771,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Benchmark-Fix Compare'!$A$3:$A$18</c:f>
+              <c:f>'Benchmark-IgnoreBackground'!$A$3:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1817,7 +1828,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Benchmark-Fix Compare'!$E$3:$E$18</c:f>
+              <c:f>'Benchmark-IgnoreBackground'!$E$3:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1825,49 +1836,49 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6420580934266096</c:v>
+                  <c:v>1.9010930418555054</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0205680389438732</c:v>
+                  <c:v>1.0918421754198882</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57264902156742636</c:v>
+                  <c:v>0.59554118901626241</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.32580031593539444</c:v>
+                  <c:v>0.33717675286590248</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.20319803991102228</c:v>
+                  <c:v>0.21837509997334045</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.14955349946806795</c:v>
+                  <c:v>0.1563249800053319</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.13108095038524775</c:v>
+                  <c:v>0.13599706744868037</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.12640639607982204</c:v>
+                  <c:v>0.12999866702212742</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.14200973596827751</c:v>
+                  <c:v>0.14666089042921887</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.18656307424481769</c:v>
+                  <c:v>0.19348173820314585</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.22766691382700927</c:v>
+                  <c:v>0.23810317248733673</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.84283826042103227</c:v>
+                  <c:v>0.88892961876832854</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.0198265579161159</c:v>
+                  <c:v>1.0965075979738739</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.0163448209162127</c:v>
+                  <c:v>1.0890429218874969</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.3870530964892485</c:v>
+                  <c:v>8.0780791788856323</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1875,7 +1886,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2227-2D47-82A7-D18DD015FC1D}"/>
+              <c16:uniqueId val="{00000000-0279-4742-B2B7-DEBAB787DE3C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1898,7 +1909,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Benchmark-Fix Compare'!$G$2</c:f>
+              <c:f>'Benchmark-IgnoreBackground'!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1933,7 +1944,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Benchmark-Fix Compare'!$A$3:$A$18</c:f>
+              <c:f>'Benchmark-IgnoreBackground'!$A$3:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1990,7 +2001,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Benchmark-Fix Compare'!$G$3:$G$18</c:f>
+              <c:f>'Benchmark-IgnoreBackground'!$G$3:$G$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1998,46 +2009,46 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55.71913075421476</c:v>
+                  <c:v>75.130377145242406</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55.716286695852901</c:v>
+                  <c:v>75.12798530346781</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>55.711188010860909</c:v>
+                  <c:v>75.120529440332277</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55.612390656014746</c:v>
+                  <c:v>74.946596950479957</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>55.394170828306606</c:v>
+                  <c:v>74.659514274832489</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>55.008148494607319</c:v>
+                  <c:v>74.361122028143001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>53.870118934010868</c:v>
+                  <c:v>72.800230865205037</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>52.406175880511945</c:v>
+                  <c:v>70.743013765614279</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50.256856579395418</c:v>
+                  <c:v>68.016750853814955</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>46.471562538433759</c:v>
+                  <c:v>62.47875510616015</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44.774903095738722</c:v>
+                  <c:v>60.272480055923516</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.5190536736438887</c:v>
+                  <c:v>11.175554652510222</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.3922938619277323</c:v>
+                  <c:v>9.6411995187386239</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.3922938619277323</c:v>
+                  <c:v>9.6411995187386239</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -2048,7 +2059,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2227-2D47-82A7-D18DD015FC1D}"/>
+              <c16:uniqueId val="{00000001-0279-4742-B2B7-DEBAB787DE3C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2423,7 +2434,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Benchmark-0'!$E$2</c:f>
+              <c:f>'Benchmark-Fix Compare'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2458,7 +2469,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Benchmark-0'!$A$3:$A$18</c:f>
+              <c:f>'Benchmark-Fix Compare'!$A$3:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2515,7 +2526,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Benchmark-0'!$E$3:$E$18</c:f>
+              <c:f>'Benchmark-Fix Compare'!$E$3:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2523,49 +2534,49 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6949940439873326</c:v>
+                  <c:v>1.6420580934266096</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0358522908858478</c:v>
+                  <c:v>1.0205680389438732</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.51390220517737295</c:v>
+                  <c:v>0.57264902156742636</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.27682384729364595</c:v>
+                  <c:v>0.32580031593539444</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.18321276039396844</c:v>
+                  <c:v>0.20319803991102228</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.14907463900752493</c:v>
+                  <c:v>0.14955349946806795</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.14773816787239608</c:v>
+                  <c:v>0.13108095038524775</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.17754728492983526</c:v>
+                  <c:v>0.12640639607982204</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.23205206426682939</c:v>
+                  <c:v>0.14200973596827751</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.35006827624277287</c:v>
+                  <c:v>0.18656307424481769</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.3986170429123449</c:v>
+                  <c:v>0.22766691382700927</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.85603881577035934</c:v>
+                  <c:v>0.84283826042103227</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.1698480490426799</c:v>
+                  <c:v>1.0198265579161159</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.0309131584299369</c:v>
+                  <c:v>1.0163448209162127</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8.755977802957668</c:v>
+                  <c:v>7.3870530964892485</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2573,7 +2584,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2803-F747-B975-326804F98C39}"/>
+              <c16:uniqueId val="{00000000-2227-2D47-82A7-D18DD015FC1D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2596,7 +2607,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Benchmark-0'!$G$2</c:f>
+              <c:f>'Benchmark-Fix Compare'!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2631,7 +2642,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Benchmark-0'!$A$3:$A$18</c:f>
+              <c:f>'Benchmark-Fix Compare'!$A$3:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2688,7 +2699,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Benchmark-0'!$G$3:$G$18</c:f>
+              <c:f>'Benchmark-Fix Compare'!$G$3:$G$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2696,46 +2707,46 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>98.404034733567556</c:v>
+                  <c:v>55.71913075421476</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>98.235459109266131</c:v>
+                  <c:v>55.716286695852901</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98.233997674220674</c:v>
+                  <c:v>55.711188010860909</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>97.013468877933761</c:v>
+                  <c:v>55.612390656014746</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>91.288483051946173</c:v>
+                  <c:v>55.394170828306606</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>90.271434597823557</c:v>
+                  <c:v>55.008148494607319</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>88.928756251136306</c:v>
+                  <c:v>53.870118934010868</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>81.024710093666101</c:v>
+                  <c:v>52.406175880511945</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>63.115721335025931</c:v>
+                  <c:v>50.256856579395418</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42.70115925125949</c:v>
+                  <c:v>46.471562538433759</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34.059361638859471</c:v>
+                  <c:v>44.774903095738722</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.4701384253723315</c:v>
+                  <c:v>8.5190536736438887</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.7941348025446291</c:v>
+                  <c:v>7.3922938619277323</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.7941348025446291</c:v>
+                  <c:v>7.3922938619277323</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -2746,7 +2757,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2803-F747-B975-326804F98C39}"/>
+              <c16:uniqueId val="{00000001-2227-2D47-82A7-D18DD015FC1D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3071,6 +3082,704 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>C Search &amp;</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> C Avg vs Max Children</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark-0'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C Search</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Benchmark-0'!$A$3:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16384</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Benchmark-0'!$E$3:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6949940439873326</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0358522908858478</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.51390220517737295</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.27682384729364595</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.18321276039396844</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.14907463900752493</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.14773816787239608</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.17754728492983526</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.23205206426682939</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.35006827624277287</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.3986170429123449</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.85603881577035934</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1698480490426799</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0309131584299369</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.755977802957668</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2803-F747-B975-326804F98C39}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="200140560"/>
+        <c:axId val="1829147359"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Benchmark-0'!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C Avg Dif</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Benchmark-0'!$A$3:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16384</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Benchmark-0'!$G$3:$G$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>98.404034733567556</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>98.235459109266131</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98.233997674220674</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97.013468877933761</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>91.288483051946173</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90.271434597823557</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>88.928756251136306</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>81.024710093666101</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>63.115721335025931</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42.70115925125949</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>34.059361638859471</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.4701384253723315</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.7941348025446291</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.7941348025446291</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2803-F747-B975-326804F98C39}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1830783935"/>
+        <c:axId val="199545920"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="200140560"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="10000"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1829147359"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1829147359"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="200140560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="199545920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1830783935"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1830783935"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="199545920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>Time</a:t>
             </a:r>
             <a:r>
@@ -3722,7 +4431,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4323,7 +5032,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5007,7 +5716,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5929,6 +6638,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -10057,7 +10806,566 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F41FEA7-ABD5-9448-9EE2-E0D506C247EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -10100,7 +11408,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -10143,7 +11451,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -10186,7 +11494,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -10227,7 +11535,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -10672,8 +11980,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7AEF0CA-7BED-8C47-B9D6-5A56E6D2CDD3}">
-  <dimension ref="A2:L18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2347A84-B413-504A-AB33-5D33B723CAFE}">
+  <dimension ref="A2:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -10705,7 +12013,7 @@
         <v>0.5</v>
       </c>
       <c r="B3">
-        <v>212.91</v>
+        <v>196.18</v>
       </c>
       <c r="C3">
         <v>1.26138969316015</v>
@@ -10731,7 +12039,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>573.04</v>
+        <v>589.17999999999995</v>
       </c>
       <c r="C4">
         <v>82.538015905202897</v>
@@ -10741,7 +12049,7 @@
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>2.691465877600864</v>
+        <v>3.0032623101233558</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
@@ -10757,7 +12065,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>329.64</v>
+        <v>340.02</v>
       </c>
       <c r="C5">
         <v>82.538015905202897</v>
@@ -10767,7 +12075,7 @@
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>1.5482598280963786</v>
+        <v>1.7332042002242836</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
@@ -10783,7 +12091,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>178.93</v>
+        <v>184.33</v>
       </c>
       <c r="C6">
         <v>82.538015905202897</v>
@@ -10793,7 +12101,7 @@
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>0.84040204781363026</v>
+        <v>0.9395962891222347</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
@@ -10809,7 +12117,7 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>100.53</v>
+        <v>106.23</v>
       </c>
       <c r="C7">
         <v>82.538015905202897</v>
@@ -10819,7 +12127,7 @@
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>0.47217134000281813</v>
+        <v>0.54149250688143546</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
@@ -10835,7 +12143,7 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>65.099999999999994</v>
+        <v>67.42</v>
       </c>
       <c r="C8">
         <v>82.538015905202897</v>
@@ -10845,7 +12153,7 @@
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>0.30576299845004928</v>
+        <v>0.34366398205729431</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
@@ -10861,7 +12169,7 @@
         <v>32</v>
       </c>
       <c r="B9">
-        <v>47.12</v>
+        <v>48.46</v>
       </c>
       <c r="C9">
         <v>82.538015905202897</v>
@@ -10871,7 +12179,7 @@
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0.22131417030670236</v>
+        <v>0.24701804465286981</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
@@ -10887,7 +12195,7 @@
         <v>64</v>
       </c>
       <c r="B10">
-        <v>41.27</v>
+        <v>42.48</v>
       </c>
       <c r="C10">
         <v>82.538015905202897</v>
@@ -10897,7 +12205,7 @@
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>0.19383777182847214</v>
+        <v>0.21653583443776123</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
@@ -10913,7 +12221,7 @@
         <v>128</v>
       </c>
       <c r="B11">
-        <v>38.6</v>
+        <v>39.46</v>
       </c>
       <c r="C11">
         <v>82.538015905202897</v>
@@ -10923,7 +12231,7 @@
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>0.18129726175379268</v>
+        <v>0.20114180854317462</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
@@ -10939,7 +12247,7 @@
         <v>256</v>
       </c>
       <c r="B12">
-        <v>43.84</v>
+        <v>45.92</v>
       </c>
       <c r="C12">
         <v>82.538015905202897</v>
@@ -10949,7 +12257,7 @@
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>0.20590859987788268</v>
+        <v>0.2340707513508003</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
@@ -10965,7 +12273,7 @@
         <v>512</v>
       </c>
       <c r="B13">
-        <v>58.48</v>
+        <v>61.64</v>
       </c>
       <c r="C13">
         <v>82.538015905202897</v>
@@ -10975,7 +12283,7 @@
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>0.27467004837724857</v>
+        <v>0.31420124375573449</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
@@ -10991,7 +12299,7 @@
         <v>1024</v>
       </c>
       <c r="B14">
-        <v>71.400000000000006</v>
+        <v>73.38</v>
       </c>
       <c r="C14">
         <v>82.538015905202897</v>
@@ -11001,7 +12309,7 @@
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>0.33535296604198961</v>
+        <v>0.374044245081048</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
@@ -11017,7 +12325,7 @@
         <v>2048</v>
       </c>
       <c r="B15">
-        <v>266.06</v>
+        <v>273.95999999999998</v>
       </c>
       <c r="C15">
         <v>55.8877226475811</v>
@@ -11027,7 +12335,7 @@
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>1.2496359964304167</v>
+        <v>1.396472627179121</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
@@ -11043,7 +12351,7 @@
         <v>4096</v>
       </c>
       <c r="B16">
-        <v>327.55</v>
+        <v>335.37</v>
       </c>
       <c r="C16">
         <v>55.8877226475811</v>
@@ -11053,7 +12361,7 @@
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>1.5384434737682591</v>
+        <v>1.7095014782342746</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
@@ -11064,12 +12372,12 @@
         <v>9.6411995187386239</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>8192</v>
       </c>
       <c r="B17">
-        <v>326.83999999999997</v>
+        <v>338.09</v>
       </c>
       <c r="C17">
         <v>55.8877226475811</v>
@@ -11079,7 +12387,7 @@
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>1.5351087313888496</v>
+        <v>1.7233662962585379</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
@@ -11091,12 +12399,12 @@
       </c>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16384</v>
       </c>
       <c r="B18" s="5">
-        <v>2422.4499999999998</v>
+        <v>2426.5500000000002</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -11106,7 +12414,7 @@
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>11.377812221126296</v>
+        <v>12.368997859108982</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
@@ -11117,6 +12425,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="5"/>
+      <c r="R18" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B4:B18">
@@ -11130,6 +12439,464 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7AEF0CA-7BED-8C47-B9D6-5A56E6D2CDD3}">
+  <dimension ref="A2:L18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0.5</v>
+      </c>
+      <c r="B3">
+        <v>212.91</v>
+      </c>
+      <c r="C3">
+        <v>1.26138969316015</v>
+      </c>
+      <c r="D3">
+        <v>6.3556460153053093E-2</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:G18" si="0">B3/B$3</f>
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>573.04</v>
+      </c>
+      <c r="C4">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D4">
+        <v>4.7750208213154499</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>2.691465877600864</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>75.130377145242406</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>329.64</v>
+      </c>
+      <c r="C5">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D5">
+        <v>4.7748688043190102</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>1.5482598280963786</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>75.12798530346781</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>178.93</v>
+      </c>
+      <c r="C6">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D6">
+        <v>4.7743949360507303</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.84040204781363026</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>75.120529440332277</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>100.53</v>
+      </c>
+      <c r="C7">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D7">
+        <v>4.7633404026901101</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.47217134000281813</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>74.946596950479957</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="C8">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D8">
+        <v>4.7450944440546898</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.30576299845004928</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>74.659514274832489</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>32</v>
+      </c>
+      <c r="B9">
+        <v>47.12</v>
+      </c>
+      <c r="C9">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D9">
+        <v>4.7261296891179896</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.22131417030670236</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>74.361122028143001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>64</v>
+      </c>
+      <c r="B10">
+        <v>41.27</v>
+      </c>
+      <c r="C10">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D10">
+        <v>4.6269249721174699</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.19383777182847214</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>72.800230865205037</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>128</v>
+      </c>
+      <c r="B11">
+        <v>38.6</v>
+      </c>
+      <c r="C11">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D11">
+        <v>4.4961755355011501</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0.18129726175379268</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>70.743013765614279</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>256</v>
+      </c>
+      <c r="B12">
+        <v>43.84</v>
+      </c>
+      <c r="C12">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D12">
+        <v>4.3229039153806301</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0.20590859987788268</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>68.016750853814955</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>512</v>
+      </c>
+      <c r="B13">
+        <v>58.48</v>
+      </c>
+      <c r="C13">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D13">
+        <v>3.9709285093170301</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0.27467004837724857</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>62.47875510616015</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1024</v>
+      </c>
+      <c r="B14">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="C14">
+        <v>82.538015905202897</v>
+      </c>
+      <c r="D14">
+        <v>3.8307054769999902</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0.33535296604198961</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>65.434192425039583</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>60.272480055923516</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2048</v>
+      </c>
+      <c r="B15">
+        <v>266.06</v>
+      </c>
+      <c r="C15">
+        <v>55.8877226475811</v>
+      </c>
+      <c r="D15">
+        <v>0.710278693960533</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>1.2496359964304167</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>44.306468453508614</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>11.175554652510222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>4096</v>
+      </c>
+      <c r="B16">
+        <v>327.55</v>
+      </c>
+      <c r="C16">
+        <v>55.8877226475811</v>
+      </c>
+      <c r="D16">
+        <v>0.61276051304034596</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>1.5384434737682591</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>44.306468453508614</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>9.6411995187386239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>8192</v>
+      </c>
+      <c r="B17">
+        <v>326.83999999999997</v>
+      </c>
+      <c r="C17">
+        <v>55.8877226475811</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0.61276051304034596</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>1.5351087313888496</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>44.306468453508614</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>9.6411995187386239</v>
+      </c>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>16384</v>
+      </c>
+      <c r="B18" s="5">
+        <v>2422.4499999999998</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>11.377812221126296</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L18" s="5"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B4:B18">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
+      <formula>$B$3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCEB006D-EF5F-2D4D-86DC-4D6E506A45E0}">
   <dimension ref="A2:L18"/>
   <sheetViews>
@@ -11586,7 +13353,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B42892-40D1-4548-A56D-9001ACB7B0BC}">
   <dimension ref="A2:I18"/>
   <sheetViews>
@@ -12059,7 +13826,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC69C5D9-B88F-FF4D-BBBE-0229262C4A41}">
   <dimension ref="A1:L18"/>
   <sheetViews>
@@ -12536,7 +14303,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393E3666-8983-354A-B652-1578FACF0E70}">
   <dimension ref="A1:G18"/>
   <sheetViews>
@@ -12997,7 +14764,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310253C2-5867-A04F-B696-06BC56F172E8}">
   <dimension ref="A1:U17"/>
   <sheetViews>

</xml_diff>